<commit_message>
feat: add ci/release automation, tests, and diagnostics improvements
</commit_message>
<xml_diff>
--- a/_docs/EnemyImbuePresets_PresetMatrix.xlsx
+++ b/_docs/EnemyImbuePresets_PresetMatrix.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Faction Profile'!$A$1:$G$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Enemy Type Profile'!$A$1:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Enemy Type Profile'!$A$1:$G$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Imbue Writes'!$A$1:$I$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Chance Writes'!$A$1:$I$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Strength Writes'!$A$1:$I$25</definedName>
@@ -547,7 +547,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Enemy Imbue Presets - Preset To Collapsible Mapping</t>
+          <t>Factioned Imbuement - Preset To Collapsible Mapping</t>
         </is>
       </c>
       <c r="B1" s="1" t="n"/>
@@ -616,12 +616,12 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Caster/Non-Caster eligibility toggles</t>
+          <t>Enemy archetype eligibility toggles</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -710,12 +710,12 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>77</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>10 eligibility toggles + 72 slot fields</t>
+          <t>5 eligibility toggles + 72 slot fields</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr"/>
@@ -757,27 +757,27 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Lore Friendly</t>
+          <t>Default</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Frontier Pressure</t>
+          <t>Core Factions</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Warfront Arcana</t>
+          <t>Most Factions</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>High Magic Conflict</t>
+          <t>All Factions</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Randomized Eligibility</t>
+          <t>Random</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
@@ -1094,7 +1094,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1120,27 +1120,27 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Lore Friendly (Casters Only)</t>
+          <t>Mage</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Frontier Pressure (Mostly Open)</t>
+          <t>Mage Bow</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Warfront Arcana (Open)</t>
+          <t>Mage Melee</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>High Magic Conflict (Open)</t>
+          <t>Mage Bow Melee</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Randomized Eligibility</t>
+          <t>Random</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
@@ -1152,7 +1152,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Caster Enemies Eligible</t>
+          <t>Mage Eligible</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -1182,49 +1182,160 @@
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t>Lore-friendly defaults caster-only; higher profiles open non-casters.</t>
+          <t>Enabled in all non-random presets.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Non-Caster Enemies Eligible</t>
+          <t>Mage Bow Eligible</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Random each apply</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>Enabled in all non-random presets.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Mage Melee Eligible</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>Random each apply</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>Enabled in all non-random presets.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Bow Eligible</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
           <t>Off</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>On</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>On</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Random each apply</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>Enabled by Mage Bow / Mage Bow Melee presets.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Melee Eligible</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>On</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>Random each apply</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>Set by Enemy Type Profile Preset; still overridable manually until preset changes.</t>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>Enabled by Mage Melee / Mage Bow Melee presets.</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G3"/>
+  <autoFilter ref="A1:G6"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1273,27 +1384,27 @@
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Lore Friendly</t>
+          <t>Default</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Frontier Doctrines</t>
+          <t>Two-Slot</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Warfront Expansion</t>
+          <t>Tri-Slot</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>High Magic Arsenal</t>
+          <t>Tri-Slot+</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Randomized</t>
+          <t>Random</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
@@ -2480,27 +2591,27 @@
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Lore Friendly</t>
+          <t>Default</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Frontier Pressure</t>
+          <t>Increased</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Warfront Arcana</t>
+          <t>High</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>High Magic Conflict</t>
+          <t>Very High</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Chaotic Storm</t>
+          <t>Maximum</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
@@ -3687,27 +3798,27 @@
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Lore Friendly</t>
+          <t>Default</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Frontier Pressure</t>
+          <t>Increased</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Warfront Arcana</t>
+          <t>High</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>High Magic Conflict</t>
+          <t>Very High</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Chaotic Storm</t>
+          <t>Maximum</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">

</xml_diff>